<commit_message>
Made the WinPt Check for the D20MX and the D20M++
Also modified the points list/rtu WinPt compare script and Excel file so it can handle a DNP DPA instance where there are more of a particular point than DNP points (because it gives an error). Just preliminary.
</commit_message>
<xml_diff>
--- a/Example D20 XML/D20MEII/D20 DNP Map WinPt Check.xlsx
+++ b/Example D20 XML/D20MEII/D20 DNP Map WinPt Check.xlsx
@@ -402,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,23 +414,23 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -438,13 +438,13 @@
       <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>4</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>1</v>
       </c>
     </row>
@@ -452,13 +452,13 @@
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>2</v>
       </c>
     </row>
@@ -466,13 +466,13 @@
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>3</v>
       </c>
     </row>
@@ -480,13 +480,13 @@
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>4</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>4</v>
       </c>
     </row>
@@ -494,13 +494,13 @@
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>5</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>5</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>5</v>
       </c>
     </row>
@@ -508,13 +508,13 @@
       <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>6</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>6</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>6</v>
       </c>
     </row>
@@ -522,13 +522,13 @@
       <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>7</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>7</v>
       </c>
     </row>
@@ -536,13 +536,13 @@
       <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>8</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>8</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>8</v>
       </c>
     </row>
@@ -550,13 +550,13 @@
       <c r="A11" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>11</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>9</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>9</v>
       </c>
     </row>
@@ -564,13 +564,13 @@
       <c r="A12" s="2">
         <v>9</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>9</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>10</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>10</v>
       </c>
     </row>
@@ -578,13 +578,13 @@
       <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>12</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>11</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>11</v>
       </c>
     </row>
@@ -592,13 +592,13 @@
       <c r="A14" s="2">
         <v>11</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>14</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>12</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>12</v>
       </c>
     </row>
@@ -606,13 +606,13 @@
       <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>10</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>13</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>13</v>
       </c>
     </row>
@@ -620,13 +620,13 @@
       <c r="A16" s="2">
         <v>13</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>13</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>14</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>14</v>
       </c>
     </row>
@@ -634,13 +634,13 @@
       <c r="A17" s="2">
         <v>14</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>19</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>15</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>15</v>
       </c>
     </row>
@@ -648,13 +648,13 @@
       <c r="A18" s="2">
         <v>15</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>20</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>16</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>16</v>
       </c>
     </row>
@@ -662,11 +662,13 @@
       <c r="A19" s="2">
         <v>16</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>21</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4">
+      <c r="C19" s="3">
+        <v>17</v>
+      </c>
+      <c r="D19" s="3">
         <v>17</v>
       </c>
     </row>
@@ -674,11 +676,13 @@
       <c r="A20" s="2">
         <v>17</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>22</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4">
+      <c r="C20" s="3">
+        <v>18</v>
+      </c>
+      <c r="D20" s="3">
         <v>18</v>
       </c>
     </row>
@@ -686,11 +690,13 @@
       <c r="A21" s="2">
         <v>18</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>16</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4">
+      <c r="C21" s="3">
+        <v>19</v>
+      </c>
+      <c r="D21" s="3">
         <v>19</v>
       </c>
     </row>
@@ -698,11 +704,13 @@
       <c r="A22" s="2">
         <v>19</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>17</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4">
+      <c r="C22" s="3">
+        <v>20</v>
+      </c>
+      <c r="D22" s="3">
         <v>20</v>
       </c>
     </row>
@@ -710,11 +718,13 @@
       <c r="A23" s="2">
         <v>20</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>15</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4">
+      <c r="C23" s="3">
+        <v>21</v>
+      </c>
+      <c r="D23" s="3">
         <v>21</v>
       </c>
     </row>
@@ -722,11 +732,13 @@
       <c r="A24" s="2">
         <v>21</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>18</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4">
+      <c r="C24" s="3">
+        <v>22</v>
+      </c>
+      <c r="D24" s="3">
         <v>22</v>
       </c>
     </row>
@@ -734,11 +746,13 @@
       <c r="A25" s="2">
         <v>22</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>29</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4">
+      <c r="C25" s="3">
+        <v>23</v>
+      </c>
+      <c r="D25" s="3">
         <v>23</v>
       </c>
     </row>
@@ -746,11 +760,13 @@
       <c r="A26" s="2">
         <v>23</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <v>30</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4">
+      <c r="C26" s="3">
+        <v>24</v>
+      </c>
+      <c r="D26" s="3">
         <v>24</v>
       </c>
     </row>
@@ -758,967 +774,935 @@
       <c r="A27" s="2">
         <v>24</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="3">
         <v>31</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="C27" s="3">
+        <v>25</v>
+      </c>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>25</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="3">
         <v>32</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+      <c r="C28" s="3">
+        <v>26</v>
+      </c>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>26</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="3">
         <v>33</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="C29" s="3">
+        <v>27</v>
+      </c>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>27</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="3">
         <v>34</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="C30" s="3">
+        <v>28</v>
+      </c>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>28</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>35</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="C31" s="3">
+        <v>29</v>
+      </c>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>29</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="3">
         <v>36</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
+      <c r="C32" s="3">
+        <v>30</v>
+      </c>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>30</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <v>37</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="C33" s="3">
+        <v>31</v>
+      </c>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>31</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="3">
         <v>38</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
+      <c r="C34" s="3">
+        <v>32</v>
+      </c>
+      <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>32</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="3">
         <v>39</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
+      <c r="C35" s="3">
+        <v>33</v>
+      </c>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>33</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="3">
         <v>40</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
+      <c r="C36" s="3">
+        <v>34</v>
+      </c>
+      <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>34</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <v>41</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
+      <c r="C37" s="3">
+        <v>35</v>
+      </c>
+      <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>35</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <v>24</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
+      <c r="C38" s="3">
+        <v>36</v>
+      </c>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>36</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B39" s="3">
         <v>23</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
+      <c r="C39" s="3">
+        <v>37</v>
+      </c>
+      <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>37</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B40" s="3">
         <v>28</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
+      <c r="C40" s="3">
+        <v>38</v>
+      </c>
+      <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>38</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="3">
         <v>25</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="C41" s="3">
+        <v>39</v>
+      </c>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>39</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B42" s="3">
         <v>26</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="C42" s="3">
+        <v>40</v>
+      </c>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>40</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="3">
         <v>27</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
+      <c r="C43" s="3">
+        <v>41</v>
+      </c>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>41</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B44" s="3">
         <v>42</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
+      <c r="C44" s="3">
+        <v>42</v>
+      </c>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>42</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B45" s="3">
         <v>43</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
+      <c r="C45" s="3">
+        <v>43</v>
+      </c>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <v>43</v>
-      </c>
-      <c r="B46" s="4">
+      <c r="A46" s="2"/>
+      <c r="B46" s="3">
         <v>44</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
+      <c r="C46" s="3">
+        <v>44</v>
+      </c>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <v>44</v>
-      </c>
-      <c r="B47" s="4">
+      <c r="A47" s="2"/>
+      <c r="B47" s="3">
         <v>45</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
+      <c r="C47" s="3">
+        <v>45</v>
+      </c>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <v>45</v>
-      </c>
-      <c r="B48" s="4">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3">
         <v>46</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
+      <c r="C48" s="3">
+        <v>46</v>
+      </c>
+      <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <v>46</v>
-      </c>
-      <c r="B49" s="4">
+      <c r="A49" s="2"/>
+      <c r="B49" s="3">
         <v>47</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
+      <c r="C49" s="3">
+        <v>47</v>
+      </c>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <v>47</v>
-      </c>
-      <c r="B50" s="4">
+      <c r="A50" s="2"/>
+      <c r="B50" s="3">
         <v>96</v>
       </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
+      <c r="C50" s="3">
+        <v>48</v>
+      </c>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <v>48</v>
-      </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3">
+        <v>49</v>
+      </c>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <v>49</v>
-      </c>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
+      <c r="A52" s="2"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
-        <v>50</v>
-      </c>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
+      <c r="A53" s="2"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
-        <v>51</v>
-      </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
+      <c r="A54" s="2"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
-        <v>52</v>
-      </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
+      <c r="A55" s="2"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
-        <v>53</v>
-      </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
+      <c r="A56" s="2"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
-        <v>54</v>
-      </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
+      <c r="A57" s="2"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="2">
-        <v>55</v>
-      </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
+      <c r="A58" s="2"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
-        <v>56</v>
-      </c>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
+      <c r="A59" s="2"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
-        <v>57</v>
-      </c>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
+      <c r="A60" s="2"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
-        <v>58</v>
-      </c>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
+      <c r="A61" s="2"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
-        <v>59</v>
-      </c>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
+      <c r="A62" s="2"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="2">
-        <v>60</v>
-      </c>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
+      <c r="A63" s="2"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="2">
-        <v>61</v>
-      </c>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
+      <c r="A64" s="2"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="2">
-        <v>62</v>
-      </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
+      <c r="A65" s="2"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
-        <v>63</v>
-      </c>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
+      <c r="A66" s="2"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
-        <v>64</v>
-      </c>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
+      <c r="A67" s="2"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="2">
-        <v>65</v>
-      </c>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
+      <c r="A68" s="2"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="2">
-        <v>66</v>
-      </c>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
+      <c r="A69" s="2"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="2">
-        <v>67</v>
-      </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
+      <c r="A70" s="2"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
-        <v>68</v>
-      </c>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
+      <c r="A71" s="2"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="2">
-        <v>69</v>
-      </c>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
+      <c r="A72" s="2"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="2">
-        <v>70</v>
-      </c>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
+      <c r="A73" s="2"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="2">
-        <v>71</v>
-      </c>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
+      <c r="A74" s="2"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="2">
-        <v>72</v>
-      </c>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
+      <c r="A75" s="2"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="2">
-        <v>73</v>
-      </c>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
+      <c r="A76" s="2"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="2">
-        <v>74</v>
-      </c>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
+      <c r="A77" s="2"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="2">
-        <v>75</v>
-      </c>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
+      <c r="A78" s="2"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="2">
-        <v>76</v>
-      </c>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
+      <c r="A79" s="2"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
-        <v>77</v>
-      </c>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
+      <c r="A80" s="2"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
-        <v>78</v>
-      </c>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
+      <c r="A81" s="2"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="2">
-        <v>79</v>
-      </c>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
+      <c r="A82" s="2"/>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="2">
-        <v>80</v>
-      </c>
-      <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4"/>
+      <c r="A83" s="2"/>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="2">
-        <v>81</v>
-      </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
+      <c r="A84" s="2"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="2">
-        <v>82</v>
-      </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
+      <c r="A85" s="2"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="2">
-        <v>83</v>
-      </c>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
+      <c r="A86" s="2"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="4"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
-      <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
-      <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="4"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="4"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
-      <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4"/>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4"/>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
-      <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
-      <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
-      <c r="B104" s="4"/>
-      <c r="C104" s="4"/>
-      <c r="D104" s="4"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
-      <c r="B105" s="4"/>
-      <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
-      <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
-      <c r="B108" s="4"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
-      <c r="B110" s="4"/>
-      <c r="C110" s="4"/>
-      <c r="D110" s="4"/>
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
-      <c r="B111" s="4"/>
-      <c r="C111" s="4"/>
-      <c r="D111" s="4"/>
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
-      <c r="B112" s="4"/>
-      <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
-      <c r="B113" s="4"/>
-      <c r="C113" s="4"/>
-      <c r="D113" s="4"/>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
-      <c r="B114" s="4"/>
-      <c r="C114" s="4"/>
-      <c r="D114" s="4"/>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
-      <c r="B115" s="4"/>
-      <c r="C115" s="4"/>
-      <c r="D115" s="4"/>
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
-      <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="4"/>
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
-      <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="4"/>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
-      <c r="B118" s="4"/>
-      <c r="C118" s="4"/>
-      <c r="D118" s="4"/>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
-      <c r="B119" s="4"/>
-      <c r="C119" s="4"/>
-      <c r="D119" s="4"/>
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
-      <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4"/>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
-      <c r="B121" s="4"/>
-      <c r="C121" s="4"/>
-      <c r="D121" s="4"/>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
-      <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="4"/>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
-      <c r="B123" s="4"/>
-      <c r="C123" s="4"/>
-      <c r="D123" s="4"/>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
-      <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
-      <c r="D124" s="4"/>
+      <c r="B124" s="3"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
-      <c r="B125" s="4"/>
-      <c r="C125" s="4"/>
-      <c r="D125" s="4"/>
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
-      <c r="B126" s="4"/>
-      <c r="C126" s="4"/>
-      <c r="D126" s="4"/>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
-      <c r="B127" s="4"/>
-      <c r="C127" s="4"/>
-      <c r="D127" s="4"/>
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
-      <c r="B128" s="4"/>
-      <c r="C128" s="4"/>
-      <c r="D128" s="4"/>
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
-      <c r="B129" s="4"/>
-      <c r="C129" s="4"/>
-      <c r="D129" s="4"/>
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
-      <c r="B130" s="4"/>
-      <c r="C130" s="4"/>
-      <c r="D130" s="4"/>
+      <c r="B130" s="3"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
-      <c r="B131" s="4"/>
-      <c r="C131" s="4"/>
-      <c r="D131" s="4"/>
+      <c r="B131" s="3"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
-      <c r="B132" s="4"/>
-      <c r="C132" s="4"/>
-      <c r="D132" s="4"/>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
-      <c r="B133" s="4"/>
-      <c r="C133" s="4"/>
-      <c r="D133" s="4"/>
+      <c r="B133" s="3"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
-      <c r="B134" s="4"/>
-      <c r="C134" s="4"/>
-      <c r="D134" s="4"/>
+      <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
-      <c r="B135" s="4"/>
-      <c r="C135" s="4"/>
-      <c r="D135" s="4"/>
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="2"/>
-      <c r="B136" s="4"/>
-      <c r="C136" s="4"/>
-      <c r="D136" s="4"/>
+      <c r="B136" s="3"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="2"/>
-      <c r="B137" s="4"/>
-      <c r="C137" s="4"/>
-      <c r="D137" s="4"/>
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="2"/>
-      <c r="B138" s="4"/>
-      <c r="C138" s="4"/>
-      <c r="D138" s="4"/>
+      <c r="B138" s="3"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="2"/>
-      <c r="B139" s="4"/>
-      <c r="C139" s="4"/>
-      <c r="D139" s="4"/>
+      <c r="B139" s="3"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="2"/>
-      <c r="B140" s="4"/>
-      <c r="C140" s="4"/>
-      <c r="D140" s="4"/>
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="2"/>
-      <c r="B141" s="4"/>
-      <c r="C141" s="4"/>
-      <c r="D141" s="4"/>
+      <c r="B141" s="3"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="2"/>
-      <c r="B142" s="4"/>
-      <c r="C142" s="4"/>
-      <c r="D142" s="4"/>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
-      <c r="B143" s="4"/>
-      <c r="C143" s="4"/>
-      <c r="D143" s="4"/>
+      <c r="B143" s="3"/>
+      <c r="C143" s="3"/>
+      <c r="D143" s="3"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="2"/>
-      <c r="B144" s="4"/>
-      <c r="C144" s="4"/>
-      <c r="D144" s="4"/>
+      <c r="B144" s="3"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="2"/>
-      <c r="B145" s="4"/>
-      <c r="C145" s="4"/>
-      <c r="D145" s="4"/>
+      <c r="B145" s="3"/>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="2"/>
-      <c r="B146" s="4"/>
-      <c r="C146" s="4"/>
-      <c r="D146" s="4"/>
+      <c r="B146" s="3"/>
+      <c r="C146" s="3"/>
+      <c r="D146" s="3"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
-      <c r="B147" s="4"/>
-      <c r="C147" s="4"/>
-      <c r="D147" s="4"/>
+      <c r="B147" s="3"/>
+      <c r="C147" s="3"/>
+      <c r="D147" s="3"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
-      <c r="B148" s="4"/>
-      <c r="C148" s="4"/>
-      <c r="D148" s="4"/>
+      <c r="B148" s="3"/>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
-      <c r="B149" s="4"/>
-      <c r="C149" s="4"/>
-      <c r="D149" s="4"/>
+      <c r="B149" s="3"/>
+      <c r="C149" s="3"/>
+      <c r="D149" s="3"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
-      <c r="B150" s="4"/>
-      <c r="C150" s="4"/>
-      <c r="D150" s="4"/>
+      <c r="B150" s="3"/>
+      <c r="C150" s="3"/>
+      <c r="D150" s="3"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
-      <c r="D151" s="4"/>
+      <c r="B151" s="3"/>
+      <c r="C151" s="3"/>
+      <c r="D151" s="3"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
-      <c r="B152" s="4"/>
-      <c r="C152" s="4"/>
-      <c r="D152" s="4"/>
+      <c r="B152" s="3"/>
+      <c r="C152" s="3"/>
+      <c r="D152" s="3"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
-      <c r="B153" s="4"/>
-      <c r="C153" s="4"/>
-      <c r="D153" s="4"/>
+      <c r="B153" s="3"/>
+      <c r="C153" s="3"/>
+      <c r="D153" s="3"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="2"/>
-      <c r="B154" s="4"/>
-      <c r="C154" s="4"/>
-      <c r="D154" s="4"/>
+      <c r="B154" s="3"/>
+      <c r="C154" s="3"/>
+      <c r="D154" s="3"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
-      <c r="B155" s="4"/>
-      <c r="C155" s="4"/>
-      <c r="D155" s="4"/>
+      <c r="B155" s="3"/>
+      <c r="C155" s="3"/>
+      <c r="D155" s="3"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="2"/>
-      <c r="B156" s="4"/>
-      <c r="C156" s="4"/>
-      <c r="D156" s="4"/>
+      <c r="B156" s="3"/>
+      <c r="C156" s="3"/>
+      <c r="D156" s="3"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
-      <c r="B157" s="4"/>
-      <c r="C157" s="4"/>
-      <c r="D157" s="4"/>
+      <c r="B157" s="3"/>
+      <c r="C157" s="3"/>
+      <c r="D157" s="3"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="2"/>
-      <c r="B158" s="4"/>
-      <c r="C158" s="4"/>
-      <c r="D158" s="4"/>
+      <c r="B158" s="3"/>
+      <c r="C158" s="3"/>
+      <c r="D158" s="3"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="2"/>
-      <c r="B159" s="4"/>
-      <c r="C159" s="4"/>
-      <c r="D159" s="4"/>
+      <c r="B159" s="3"/>
+      <c r="C159" s="3"/>
+      <c r="D159" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Bug Fixes for WinPt Check
Added an if statment to handle if a WinPt was undefined on the SGConfig XML.
Added an if statment to handle if the excel sheet runs out of WinPt's before the SGConfig
</commit_message>
<xml_diff>
--- a/Example D20 XML/D20MEII/D20 DNP Map WinPt Check.xlsx
+++ b/Example D20 XML/D20MEII/D20 DNP Map WinPt Check.xlsx
@@ -402,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -999,7 +999,9 @@
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="2"/>
+      <c r="A46" s="2">
+        <v>43</v>
+      </c>
       <c r="B46" s="3">
         <v>44</v>
       </c>
@@ -1009,7 +1011,9 @@
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
+      <c r="A47" s="2">
+        <v>44</v>
+      </c>
       <c r="B47" s="3">
         <v>45</v>
       </c>
@@ -1019,7 +1023,9 @@
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="2"/>
+      <c r="A48" s="2">
+        <v>45</v>
+      </c>
       <c r="B48" s="3">
         <v>46</v>
       </c>
@@ -1029,7 +1035,9 @@
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="2"/>
+      <c r="A49" s="2">
+        <v>46</v>
+      </c>
       <c r="B49" s="3">
         <v>47</v>
       </c>
@@ -1039,7 +1047,9 @@
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="2"/>
+      <c r="A50" s="2">
+        <v>47</v>
+      </c>
       <c r="B50" s="3">
         <v>96</v>
       </c>
@@ -1049,7 +1059,9 @@
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="2"/>
+      <c r="A51" s="2">
+        <v>48</v>
+      </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3">
         <v>49</v>
@@ -1057,37 +1069,49 @@
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="2"/>
+      <c r="A52" s="2">
+        <v>49</v>
+      </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="2"/>
+      <c r="A53" s="2">
+        <v>50</v>
+      </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="2"/>
+      <c r="A54" s="2">
+        <v>51</v>
+      </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="2"/>
+      <c r="A55" s="2">
+        <v>52</v>
+      </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="2"/>
+      <c r="A56" s="2">
+        <v>53</v>
+      </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="2"/>
+      <c r="A57" s="2">
+        <v>54</v>
+      </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>

</xml_diff>